<commit_message>
Need fix bug with edit form
</commit_message>
<xml_diff>
--- a/Книга1.xlsx
+++ b/Книга1.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\работа\шаблоны\Новая папка\calendar\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\myProgects\calendar\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="38">
   <si>
     <t>Не закрывается форма с полями обязательными для заполнения</t>
   </si>
@@ -134,7 +134,10 @@
     <t>не работает в chome, найти как генерить на сервере less файл и отдавать на клиент css</t>
   </si>
   <si>
-    <t>если просматривать несколько подряд событий,а потом исправить одно,то правки во всех просмотренных и так же добавляется одно лишнее событие</t>
+    <t>не удаляет и не правит событие</t>
+  </si>
+  <si>
+    <t>почему-то event после того,как форма открывается, обнуляется undefined</t>
   </si>
 </sst>
 </file>
@@ -678,16 +681,16 @@
   <dimension ref="A1:D23"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="B21" sqref="B21"/>
+      <selection activeCell="A23" sqref="A23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="2" max="2" width="69.85546875" customWidth="1"/>
-    <col min="3" max="3" width="106.85546875" customWidth="1"/>
+    <col min="2" max="2" width="69.81640625" customWidth="1"/>
+    <col min="3" max="3" width="106.81640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="31.5" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" ht="31.5" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A1" s="1">
         <v>1</v>
       </c>
@@ -698,7 +701,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:4" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:4" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A2" s="3">
         <v>2</v>
       </c>
@@ -707,7 +710,7 @@
       </c>
       <c r="C2" s="4"/>
     </row>
-    <row r="3" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A3" s="3">
         <v>3</v>
       </c>
@@ -718,7 +721,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="1:4" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:4" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A4" s="3">
         <v>4</v>
       </c>
@@ -729,7 +732,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="5" spans="1:4" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:4" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A5" s="3">
         <v>5</v>
       </c>
@@ -738,7 +741,7 @@
       </c>
       <c r="C5" s="4"/>
     </row>
-    <row r="6" spans="1:4" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:4" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A6" s="3">
         <v>6</v>
       </c>
@@ -749,7 +752,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="7" spans="1:4" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:4" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A7" s="13">
         <v>7</v>
       </c>
@@ -760,7 +763,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="8" spans="1:4" ht="17.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:4" ht="17.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A8" s="5">
         <v>8</v>
       </c>
@@ -769,7 +772,7 @@
       </c>
       <c r="C8" s="4"/>
     </row>
-    <row r="9" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A9" s="3">
         <v>9</v>
       </c>
@@ -778,7 +781,7 @@
       </c>
       <c r="C9" s="4"/>
     </row>
-    <row r="10" spans="1:4" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:4" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A10" s="3">
         <v>10</v>
       </c>
@@ -789,7 +792,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="11" spans="1:4" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:4" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A11" s="3">
         <v>11</v>
       </c>
@@ -800,7 +803,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="12" spans="1:4" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:4" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A12" s="19">
         <v>12</v>
       </c>
@@ -812,7 +815,7 @@
       </c>
       <c r="D12" s="18"/>
     </row>
-    <row r="13" spans="1:4" ht="21" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:4" ht="21" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A13" s="8">
         <v>13</v>
       </c>
@@ -823,7 +826,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="14" spans="1:4" ht="17.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:4" ht="17.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A14" s="8">
         <v>14</v>
       </c>
@@ -834,7 +837,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="15" spans="1:4" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:4" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A15" s="8">
         <v>15</v>
       </c>
@@ -843,7 +846,7 @@
       </c>
       <c r="C15" s="9"/>
     </row>
-    <row r="16" spans="1:4" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:4" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A16" s="14">
         <v>16</v>
       </c>
@@ -854,7 +857,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A17" s="16">
         <v>17</v>
       </c>
@@ -866,7 +869,7 @@
       </c>
       <c r="D17" s="18"/>
     </row>
-    <row r="18" spans="1:4" ht="26.25" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:4" ht="26" x14ac:dyDescent="0.35">
       <c r="A18" s="12">
         <v>18</v>
       </c>
@@ -874,7 +877,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="19" spans="1:4" ht="26.25" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:4" ht="26" x14ac:dyDescent="0.35">
       <c r="A19" s="20">
         <v>19</v>
       </c>
@@ -884,7 +887,7 @@
       <c r="C19" s="10"/>
       <c r="D19" s="20"/>
     </row>
-    <row r="20" spans="1:4" ht="26.25" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:4" ht="26" x14ac:dyDescent="0.35">
       <c r="A20" s="20">
         <v>20</v>
       </c>
@@ -896,7 +899,7 @@
       </c>
       <c r="D20" s="17"/>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A21" s="11">
         <v>21</v>
       </c>
@@ -908,7 +911,7 @@
       </c>
       <c r="D21" s="11"/>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A22" s="11">
         <v>22</v>
       </c>
@@ -917,12 +920,15 @@
       </c>
       <c r="D22" s="11"/>
     </row>
-    <row r="23" spans="1:4" ht="26.25" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A23" s="11">
         <v>23</v>
       </c>
       <c r="B23" s="10" t="s">
         <v>36</v>
+      </c>
+      <c r="C23" t="s">
+        <v>37</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
work fine exsept IE
</commit_message>
<xml_diff>
--- a/Книга1.xlsx
+++ b/Книга1.xlsx
@@ -104,9 +104,6 @@
     <t>при правке события</t>
   </si>
   <si>
-    <t>при выборе в поиске показывать событие</t>
-  </si>
-  <si>
     <t>при всплытии формы,если до этого было добавлено событие,то будут поля заполнены</t>
   </si>
   <si>
@@ -125,9 +122,6 @@
     <t>script.js:175:29 появляется каждый раз после закрытия формы</t>
   </si>
   <si>
-    <t>показываем месяц с этим событием вызвать событие клик на этой дате</t>
-  </si>
-  <si>
     <t>включить проверку не отключен ли в баузере js</t>
   </si>
   <si>
@@ -138,6 +132,12 @@
   </si>
   <si>
     <t>почему-то event после того,как форма открывается, обнуляется undefined</t>
+  </si>
+  <si>
+    <t>основа проблемы с обязательными полями</t>
+  </si>
+  <si>
+    <t>при изменении и добавлении события обновляется открывается текущий месяц</t>
   </si>
 </sst>
 </file>
@@ -214,7 +214,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="9">
+  <borders count="8">
     <border>
       <left/>
       <right/>
@@ -327,23 +327,12 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left style="medium">
-        <color rgb="FFCCCCCC"/>
-      </left>
-      <right style="medium">
-        <color rgb="FFCCCCCC"/>
-      </right>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" wrapText="1"/>
@@ -357,9 +346,6 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -385,18 +371,15 @@
     <xf numFmtId="0" fontId="1" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Гиперссылка" xfId="1" builtinId="8"/>
@@ -678,10 +661,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D23"/>
+  <dimension ref="A1:D24"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="A23" sqref="A23"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B19" sqref="B19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -753,7 +736,7 @@
       </c>
     </row>
     <row r="7" spans="1:4" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A7" s="13">
+      <c r="A7" s="12">
         <v>7</v>
       </c>
       <c r="B7" s="4" t="s">
@@ -764,7 +747,7 @@
       </c>
     </row>
     <row r="8" spans="1:4" ht="17.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A8" s="5">
+      <c r="A8" s="12">
         <v>8</v>
       </c>
       <c r="B8" s="4" t="s">
@@ -804,130 +787,134 @@
       </c>
     </row>
     <row r="12" spans="1:4" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A12" s="19">
+      <c r="A12" s="18">
         <v>12</v>
       </c>
-      <c r="B12" s="6" t="s">
+      <c r="B12" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="C12" s="7" t="s">
+      <c r="C12" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="D12" s="15"/>
+    </row>
+    <row r="13" spans="1:4" ht="21" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A13" s="7">
+        <v>13</v>
+      </c>
+      <c r="B13" s="8" t="s">
+        <v>19</v>
+      </c>
+      <c r="C13" s="8" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" ht="17.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A14" s="7">
+        <v>14</v>
+      </c>
+      <c r="B14" s="8" t="s">
+        <v>21</v>
+      </c>
+      <c r="C14" s="8" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A15" s="7">
+        <v>15</v>
+      </c>
+      <c r="B15" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="C15" s="8"/>
+    </row>
+    <row r="16" spans="1:4" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A16" s="13">
+        <v>16</v>
+      </c>
+      <c r="B16" s="8" t="s">
+        <v>24</v>
+      </c>
+      <c r="C16" s="8" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" ht="26" x14ac:dyDescent="0.35">
+      <c r="A17" s="11">
+        <v>18</v>
+      </c>
+      <c r="B17" s="9" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" ht="26" x14ac:dyDescent="0.35">
+      <c r="A18" s="16">
+        <v>19</v>
+      </c>
+      <c r="B18" s="9" t="s">
+        <v>27</v>
+      </c>
+      <c r="C18" s="9"/>
+      <c r="D18" s="16"/>
+    </row>
+    <row r="19" spans="1:4" ht="26" x14ac:dyDescent="0.35">
+      <c r="A19" s="16">
+        <v>20</v>
+      </c>
+      <c r="B19" s="9" t="s">
+        <v>28</v>
+      </c>
+      <c r="C19" t="s">
+        <v>29</v>
+      </c>
+      <c r="D19" s="14"/>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A20" s="16">
+        <v>21</v>
+      </c>
+      <c r="B20" t="s">
+        <v>30</v>
+      </c>
+      <c r="C20" t="s">
+        <v>31</v>
+      </c>
+      <c r="D20" s="10"/>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A21" s="16">
+        <v>22</v>
+      </c>
+      <c r="B21" s="9" t="s">
+        <v>32</v>
+      </c>
+      <c r="D21" s="10"/>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A22" s="16">
+        <v>23</v>
+      </c>
+      <c r="B22" s="9" t="s">
+        <v>34</v>
+      </c>
+      <c r="C22" t="s">
         <v>35</v>
       </c>
-      <c r="D12" s="18"/>
-    </row>
-    <row r="13" spans="1:4" ht="21" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A13" s="8">
-        <v>13</v>
-      </c>
-      <c r="B13" s="9" t="s">
-        <v>19</v>
-      </c>
-      <c r="C13" s="9" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" ht="17.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A14" s="8">
-        <v>14</v>
-      </c>
-      <c r="B14" s="9" t="s">
-        <v>21</v>
-      </c>
-      <c r="C14" s="9" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A15" s="8">
-        <v>15</v>
-      </c>
-      <c r="B15" s="9" t="s">
-        <v>23</v>
-      </c>
-      <c r="C15" s="9"/>
-    </row>
-    <row r="16" spans="1:4" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A16" s="14">
-        <v>16</v>
-      </c>
-      <c r="B16" s="9" t="s">
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A23" s="16">
         <v>24</v>
       </c>
-      <c r="C16" s="9" t="s">
+      <c r="B23" s="17" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A24" s="16">
         <v>25</v>
       </c>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A17" s="16">
-        <v>17</v>
-      </c>
-      <c r="B17" s="10" t="s">
-        <v>26</v>
-      </c>
-      <c r="C17" s="15" t="s">
-        <v>33</v>
-      </c>
-      <c r="D17" s="18"/>
-    </row>
-    <row r="18" spans="1:4" ht="26" x14ac:dyDescent="0.35">
-      <c r="A18" s="12">
-        <v>18</v>
-      </c>
-      <c r="B18" s="10" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4" ht="26" x14ac:dyDescent="0.35">
-      <c r="A19" s="20">
-        <v>19</v>
-      </c>
-      <c r="B19" s="10" t="s">
-        <v>28</v>
-      </c>
-      <c r="C19" s="10"/>
-      <c r="D19" s="20"/>
-    </row>
-    <row r="20" spans="1:4" ht="26" x14ac:dyDescent="0.35">
-      <c r="A20" s="20">
-        <v>20</v>
-      </c>
-      <c r="B20" s="10" t="s">
-        <v>29</v>
-      </c>
-      <c r="C20" t="s">
-        <v>30</v>
-      </c>
-      <c r="D20" s="17"/>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A21" s="11">
-        <v>21</v>
-      </c>
-      <c r="B21" t="s">
-        <v>31</v>
-      </c>
-      <c r="C21" t="s">
-        <v>32</v>
-      </c>
-      <c r="D21" s="11"/>
-    </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A22" s="11">
-        <v>22</v>
-      </c>
-      <c r="B22" s="10" t="s">
-        <v>34</v>
-      </c>
-      <c r="D22" s="11"/>
-    </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A23" s="11">
-        <v>23</v>
-      </c>
-      <c r="B23" s="10" t="s">
-        <v>36</v>
-      </c>
-      <c r="C23" t="s">
+      <c r="B24" s="9" t="s">
         <v>37</v>
       </c>
     </row>

</xml_diff>